<commit_message>
kept working on script to write ROM files
</commit_message>
<xml_diff>
--- a/tool-defs/ndi_rom_format.xlsx
+++ b/tool-defs/ndi_rom_format.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="259">
   <si>
     <t>YEAR</t>
   </si>
@@ -84,9 +84,6 @@
     <t># MARKERS</t>
   </si>
   <si>
-    <t>MIN MARKERS</t>
-  </si>
-  <si>
     <t>MAX 3D ERROR</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>MIN SPREAD 3</t>
   </si>
   <si>
-    <t>CHKSUM (7:end)</t>
-  </si>
-  <si>
     <t>A normal (x)</t>
   </si>
   <si>
@@ -784,13 +778,37 @@
   </si>
   <si>
     <t>Unknown: set to 0x00</t>
+  </si>
+  <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>Not sure what the 0x01 in byte 8 represents…</t>
+  </si>
+  <si>
+    <t>CHKSUM of 7:end</t>
+  </si>
+  <si>
+    <t>MIN MKRS</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>0x41</t>
+  </si>
+  <si>
+    <t>Not sure what 0x20 and 0x41 represent…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -878,6 +896,21 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1025,7 +1058,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1037,6 +1070,96 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1064,77 +1187,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1422,1746 +1480,1839 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:F8"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21:N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" customWidth="1"/>
-    <col min="15" max="15" width="10.21875" customWidth="1"/>
-    <col min="18" max="18" width="10.33203125" customWidth="1"/>
-    <col min="20" max="20" width="114.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="0" style="16" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="8.88671875" style="26"/>
+    <col min="12" max="12" width="10.77734375" style="26" customWidth="1"/>
+    <col min="13" max="14" width="8.88671875" style="26"/>
+    <col min="15" max="15" width="10.21875" style="26" customWidth="1"/>
+    <col min="16" max="17" width="8.88671875" style="26"/>
+    <col min="18" max="18" width="10.33203125" style="26" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" style="16"/>
+    <col min="20" max="20" width="114.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29">
-        <v>0</v>
-      </c>
-      <c r="D1" s="29">
-        <v>1</v>
-      </c>
-      <c r="E1" s="29">
+    <row r="1" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13">
+        <v>1</v>
+      </c>
+      <c r="E1" s="13">
         <v>2</v>
       </c>
-      <c r="F1" s="29">
+      <c r="F1" s="13">
         <v>3</v>
       </c>
-      <c r="G1" s="29">
+      <c r="G1" s="13">
         <v>4</v>
       </c>
-      <c r="H1" s="29">
+      <c r="H1" s="13">
         <v>5</v>
       </c>
-      <c r="I1" s="29">
+      <c r="I1" s="13">
         <v>6</v>
       </c>
-      <c r="J1" s="29">
+      <c r="J1" s="13">
         <v>7</v>
       </c>
-      <c r="K1" s="29">
+      <c r="K1" s="13">
         <v>8</v>
       </c>
-      <c r="L1" s="29">
+      <c r="L1" s="13">
         <v>9</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="N1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="O1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="29" t="s">
+      <c r="Q1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="R1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="44" t="s">
-        <v>151</v>
+      <c r="T1" s="15" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="26" t="str">
+      <c r="A2" s="16">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13" t="str">
         <f>"0x"&amp;DEC2HEX(A2,8)</f>
         <v>0x00000000</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="50"/>
-      <c r="G2" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="23" t="s">
+      <c r="F2" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="H2" s="31"/>
+      <c r="I2" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="O2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="23" t="s">
+      <c r="P2" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="R2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="T2" t="s">
-        <v>152</v>
+      <c r="T2" s="16" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="16">
         <v>16</v>
       </c>
-      <c r="B3" s="26" t="str">
+      <c r="B3" s="13" t="str">
         <f>"0x"&amp;DEC2HEX(A3,8)</f>
         <v>0x00000010</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="23" t="s">
+      <c r="D3" s="27"/>
+      <c r="E3" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="23" t="s">
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="20"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="23" t="s">
+      <c r="L3" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="O3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="T3" t="s">
-        <v>153</v>
+      <c r="P3" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="16">
         <v>32</v>
       </c>
-      <c r="B4" s="26" t="str">
+      <c r="B4" s="13" t="str">
         <f t="shared" ref="B4:B21" si="0">"0x"&amp;DEC2HEX(A4,8)</f>
         <v>0x00000020</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="G4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="25" t="s">
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25" t="s">
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="T4" t="s">
-        <v>154</v>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="T4" s="16" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="16">
         <v>48</v>
       </c>
-      <c r="B5" s="26" t="str">
+      <c r="B5" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x00000030</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
+      <c r="C5" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="16">
         <v>64</v>
       </c>
-      <c r="B6" s="26" t="str">
+      <c r="B6" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x00000040</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="38" t="s">
-        <v>175</v>
-      </c>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="40"/>
-      <c r="T6" t="s">
-        <v>250</v>
+      <c r="C6" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="30"/>
+      <c r="T6" s="16" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="16">
         <v>80</v>
       </c>
-      <c r="B7" s="26" t="str">
+      <c r="B7" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x00000050</v>
       </c>
-      <c r="C7" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="38" t="s">
-        <v>156</v>
-      </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="38" t="s">
-        <v>176</v>
-      </c>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="40"/>
-      <c r="T7" t="s">
-        <v>251</v>
+      <c r="C7" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="30"/>
+      <c r="T7" s="16" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="16">
         <v>96</v>
       </c>
-      <c r="B8" s="26" t="str">
+      <c r="B8" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x00000060</v>
       </c>
-      <c r="C8" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="38" t="s">
-        <v>177</v>
-      </c>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="38" t="s">
-        <v>158</v>
-      </c>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="40"/>
+      <c r="C8" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="30"/>
+      <c r="T8" s="16" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="16">
         <v>112</v>
       </c>
-      <c r="B9" s="26" t="str">
+      <c r="B9" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x00000070</v>
       </c>
-      <c r="C9" s="38" t="s">
-        <v>178</v>
-      </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="38" t="s">
-        <v>198</v>
-      </c>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="38" t="s">
-        <v>179</v>
-      </c>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="40"/>
+      <c r="C9" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="30"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="16">
         <v>128</v>
       </c>
-      <c r="B10" s="26" t="str">
+      <c r="B10" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x00000080</v>
       </c>
-      <c r="C10" s="38" t="s">
-        <v>199</v>
-      </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="38" t="s">
-        <v>200</v>
-      </c>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="40"/>
+      <c r="C10" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="30"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="16">
         <v>144</v>
       </c>
-      <c r="B11" s="26" t="str">
+      <c r="B11" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x00000090</v>
       </c>
-      <c r="C11" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="38" t="s">
-        <v>201</v>
-      </c>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="40"/>
+      <c r="C11" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="30"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="16">
         <v>160</v>
       </c>
-      <c r="B12" s="26" t="str">
+      <c r="B12" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x000000A0</v>
       </c>
-      <c r="C12" s="38" t="s">
-        <v>182</v>
-      </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="38" t="s">
-        <v>202</v>
-      </c>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="40"/>
-      <c r="O12" s="38" t="s">
-        <v>183</v>
-      </c>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="40"/>
+      <c r="C12" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="30"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="16">
         <v>176</v>
       </c>
-      <c r="B13" s="26" t="str">
+      <c r="B13" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x000000B0</v>
       </c>
-      <c r="C13" s="38" t="s">
-        <v>203</v>
-      </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="38" t="s">
-        <v>184</v>
-      </c>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="40"/>
-      <c r="O13" s="38" t="s">
-        <v>204</v>
-      </c>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="40"/>
+      <c r="C13" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="30"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="16">
         <v>192</v>
       </c>
-      <c r="B14" s="26" t="str">
+      <c r="B14" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x000000C0</v>
       </c>
-      <c r="C14" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="38" t="s">
-        <v>185</v>
-      </c>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="38" t="s">
-        <v>205</v>
-      </c>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="38" t="s">
-        <v>166</v>
-      </c>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="40"/>
+      <c r="C14" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="30"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="16">
         <v>208</v>
       </c>
-      <c r="B15" s="26" t="str">
+      <c r="B15" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x000000D0</v>
       </c>
-      <c r="C15" s="38" t="s">
-        <v>186</v>
-      </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="38" t="s">
-        <v>187</v>
-      </c>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="40"/>
+      <c r="C15" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="30"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="16">
         <v>224</v>
       </c>
-      <c r="B16" s="26" t="str">
+      <c r="B16" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x000000E0</v>
       </c>
-      <c r="C16" s="38" t="s">
-        <v>207</v>
-      </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="38" t="s">
-        <v>168</v>
-      </c>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="38" t="s">
-        <v>188</v>
-      </c>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="38" t="s">
-        <v>208</v>
-      </c>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="40"/>
+      <c r="C16" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="30"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="16">
         <v>240</v>
       </c>
-      <c r="B17" s="26" t="str">
+      <c r="B17" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x000000F0</v>
       </c>
-      <c r="C17" s="38" t="s">
-        <v>169</v>
-      </c>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="38" t="s">
-        <v>189</v>
-      </c>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="38" t="s">
-        <v>209</v>
-      </c>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="38" t="s">
-        <v>170</v>
-      </c>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="40"/>
+      <c r="C17" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="30"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="16">
         <v>256</v>
       </c>
-      <c r="B18" s="26" t="str">
+      <c r="B18" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x00000100</v>
       </c>
-      <c r="C18" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="38" t="s">
-        <v>210</v>
-      </c>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="38" t="s">
-        <v>171</v>
-      </c>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="40"/>
-      <c r="O18" s="38" t="s">
-        <v>191</v>
-      </c>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="39"/>
-      <c r="R18" s="40"/>
+      <c r="C18" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="30"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="16">
         <v>272</v>
       </c>
-      <c r="B19" s="26" t="str">
+      <c r="B19" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x00000110</v>
       </c>
-      <c r="C19" s="38" t="s">
-        <v>211</v>
-      </c>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="38" t="s">
-        <v>172</v>
-      </c>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="38" t="s">
-        <v>192</v>
-      </c>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="38" t="s">
-        <v>212</v>
-      </c>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="39"/>
-      <c r="R19" s="40"/>
+      <c r="C19" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="30"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="16">
         <v>288</v>
       </c>
-      <c r="B20" s="26" t="str">
+      <c r="B20" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x00000120</v>
       </c>
-      <c r="C20" s="38" t="s">
-        <v>173</v>
-      </c>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="40"/>
+      <c r="C20" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="30"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="16">
         <v>304</v>
       </c>
-      <c r="B21" s="26" t="str">
+      <c r="B21" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0x00000130</v>
       </c>
-      <c r="C21" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="38" t="s">
-        <v>214</v>
-      </c>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="43"/>
-      <c r="O21" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="43"/>
+      <c r="C21" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="P21" s="33"/>
+      <c r="Q21" s="33"/>
+      <c r="R21" s="34"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="16">
         <v>320</v>
       </c>
-      <c r="B22" s="26" t="str">
+      <c r="B22" s="13" t="str">
         <f>"0x"&amp;DEC2HEX(A22,8)</f>
         <v>0x00000140</v>
       </c>
-      <c r="C22" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="43"/>
+      <c r="C22" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="33"/>
+      <c r="R22" s="34"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="16">
         <v>336</v>
       </c>
-      <c r="B23" s="26" t="str">
+      <c r="B23" s="13" t="str">
         <f>"0x"&amp;DEC2HEX(A23,8)</f>
         <v>0x00000150</v>
       </c>
-      <c r="C23" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="42"/>
-      <c r="R23" s="43"/>
+      <c r="C23" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="P23" s="33"/>
+      <c r="Q23" s="33"/>
+      <c r="R23" s="34"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="A24" s="16">
         <v>352</v>
       </c>
-      <c r="B24" s="26" t="str">
+      <c r="B24" s="13" t="str">
         <f t="shared" ref="B24:B31" si="1">"0x"&amp;DEC2HEX(A24,8)</f>
         <v>0x00000160</v>
       </c>
-      <c r="C24" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="43"/>
+      <c r="C24" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="33"/>
+      <c r="R24" s="34"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="A25" s="16">
         <v>368</v>
       </c>
-      <c r="B25" s="26" t="str">
+      <c r="B25" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0x00000170</v>
       </c>
-      <c r="C25" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="43"/>
+      <c r="C25" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="33"/>
+      <c r="R25" s="34"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="16">
         <v>384</v>
       </c>
-      <c r="B26" s="26" t="str">
+      <c r="B26" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0x00000180</v>
       </c>
-      <c r="C26" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="43"/>
+      <c r="C26" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="P26" s="33"/>
+      <c r="Q26" s="33"/>
+      <c r="R26" s="34"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="16">
         <v>400</v>
       </c>
-      <c r="B27" s="26" t="str">
+      <c r="B27" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0x00000190</v>
       </c>
-      <c r="C27" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="43"/>
+      <c r="C27" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="P27" s="33"/>
+      <c r="Q27" s="33"/>
+      <c r="R27" s="34"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="16">
         <v>416</v>
       </c>
-      <c r="B28" s="26" t="str">
+      <c r="B28" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0x000001A0</v>
       </c>
-      <c r="C28" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="L28" s="42"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="43"/>
-      <c r="O28" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="42"/>
-      <c r="R28" s="43"/>
+      <c r="C28" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="33"/>
+      <c r="R28" s="34"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="16">
         <v>432</v>
       </c>
-      <c r="B29" s="26" t="str">
+      <c r="B29" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0x000001B0</v>
       </c>
-      <c r="C29" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="L29" s="42"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="43"/>
-      <c r="O29" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="P29" s="42"/>
-      <c r="Q29" s="42"/>
-      <c r="R29" s="43"/>
+      <c r="C29" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="34"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="A30" s="16">
         <v>448</v>
       </c>
-      <c r="B30" s="26" t="str">
+      <c r="B30" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0x000001C0</v>
       </c>
-      <c r="C30" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="P30" s="42"/>
-      <c r="Q30" s="42"/>
-      <c r="R30" s="43"/>
+      <c r="C30" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="P30" s="33"/>
+      <c r="Q30" s="33"/>
+      <c r="R30" s="34"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="A31" s="16">
         <v>464</v>
       </c>
-      <c r="B31" s="26" t="str">
+      <c r="B31" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0x000001D0</v>
       </c>
-      <c r="C31" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="L31" s="42"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="P31" s="42"/>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="43"/>
+      <c r="C31" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="P31" s="33"/>
+      <c r="Q31" s="33"/>
+      <c r="R31" s="34"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="A32" s="16">
         <v>480</v>
       </c>
-      <c r="B32" s="26" t="str">
+      <c r="B32" s="13" t="str">
         <f>"0x"&amp;DEC2HEX(A32,8)</f>
         <v>0x000001E0</v>
       </c>
-      <c r="C32" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="L32" s="42"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="43"/>
-      <c r="O32" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="P32" s="42"/>
-      <c r="Q32" s="42"/>
-      <c r="R32" s="43"/>
+      <c r="C32" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="34"/>
+      <c r="O32" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="P32" s="33"/>
+      <c r="Q32" s="33"/>
+      <c r="R32" s="34"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="A33" s="16">
         <v>496</v>
       </c>
-      <c r="B33" s="26" t="str">
+      <c r="B33" s="13" t="str">
         <f>"0x"&amp;DEC2HEX(A33,8)</f>
         <v>0x000001F0</v>
       </c>
-      <c r="C33" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="L33" s="42"/>
-      <c r="M33" s="42"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="P33" s="42"/>
-      <c r="Q33" s="42"/>
-      <c r="R33" s="43"/>
+      <c r="C33" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="34"/>
+      <c r="O33" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="P33" s="33"/>
+      <c r="Q33" s="33"/>
+      <c r="R33" s="34"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="A34" s="16">
         <v>512</v>
       </c>
-      <c r="B34" s="26" t="str">
+      <c r="B34" s="13" t="str">
         <f t="shared" ref="B34:B43" si="2">"0x"&amp;DEC2HEX(A34,8)</f>
         <v>0x00000200</v>
       </c>
-      <c r="C34" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="L34" s="42"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="43"/>
-      <c r="O34" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="P34" s="42"/>
-      <c r="Q34" s="42"/>
-      <c r="R34" s="43"/>
+      <c r="C34" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="L34" s="33"/>
+      <c r="M34" s="33"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="P34" s="33"/>
+      <c r="Q34" s="33"/>
+      <c r="R34" s="34"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="16">
         <v>528</v>
       </c>
-      <c r="B35" s="26" t="str">
+      <c r="B35" s="13" t="str">
         <f t="shared" si="2"/>
         <v>0x00000210</v>
       </c>
-      <c r="C35" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="L35" s="42"/>
-      <c r="M35" s="42"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="P35" s="42"/>
-      <c r="Q35" s="42"/>
-      <c r="R35" s="43"/>
+      <c r="C35" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="34"/>
+      <c r="O35" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="P35" s="33"/>
+      <c r="Q35" s="33"/>
+      <c r="R35" s="34"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="16">
         <v>544</v>
       </c>
-      <c r="B36" s="26" t="str">
+      <c r="B36" s="13" t="str">
         <f t="shared" si="2"/>
         <v>0x00000220</v>
       </c>
-      <c r="C36" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="41" t="s">
+      <c r="C36" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="L36" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="34" t="s">
+      <c r="M36" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="L36" s="34" t="s">
+      <c r="N36" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="M36" s="34" t="s">
+      <c r="O36" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="N36" s="34" t="s">
+      <c r="P36" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="O36" s="34" t="s">
+      <c r="Q36" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="P36" s="34" t="s">
+      <c r="R36" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="Q36" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="R36" s="34" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="A37" s="16">
         <v>560</v>
       </c>
-      <c r="B37" s="26" t="str">
+      <c r="B37" s="13" t="str">
         <f t="shared" si="2"/>
         <v>0x00000230</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C37" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="D37" s="34" t="s">
+      <c r="F37" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="34" t="s">
+      <c r="G37" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="F37" s="34" t="s">
+      <c r="H37" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="G37" s="34" t="s">
+      <c r="I37" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="H37" s="34" t="s">
+      <c r="J37" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="I37" s="34" t="s">
+      <c r="K37" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="J37" s="34" t="s">
+      <c r="L37" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="K37" s="34" t="s">
+      <c r="M37" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="L37" s="34" t="s">
+      <c r="N37" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="M37" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="N37" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="O37" s="45" t="s">
+      <c r="O37" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="P37" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="P37" s="45" t="s">
+      <c r="Q37" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="R37" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="Q37" s="45" t="s">
-        <v>218</v>
-      </c>
-      <c r="R37" s="45" t="s">
-        <v>219</v>
-      </c>
-      <c r="T37" t="s">
-        <v>216</v>
+      <c r="T37" s="16" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="16">
         <v>576</v>
       </c>
-      <c r="B38" s="26" t="str">
+      <c r="B38" s="13" t="str">
         <f t="shared" si="2"/>
         <v>0x00000240</v>
       </c>
-      <c r="C38" s="46" t="s">
+      <c r="C38" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="E38" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="D38" s="46" t="s">
+      <c r="F38" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="E38" s="46" t="s">
+      <c r="G38" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="36"/>
+      <c r="L38" s="36"/>
+      <c r="M38" s="36"/>
+      <c r="N38" s="36"/>
+      <c r="O38" s="36"/>
+      <c r="P38" s="36"/>
+      <c r="Q38" s="36"/>
+      <c r="R38" s="37"/>
+      <c r="T38" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="F38" s="46" t="s">
-        <v>223</v>
-      </c>
-      <c r="G38" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
-      <c r="Q38" s="32"/>
-      <c r="R38" s="33"/>
-      <c r="T38" t="s">
-        <v>224</v>
-      </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="A39" s="16">
         <v>592</v>
       </c>
-      <c r="B39" s="26" t="str">
+      <c r="B39" s="13" t="str">
         <f t="shared" si="2"/>
         <v>0x00000250</v>
       </c>
-      <c r="C39" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
-      <c r="P39" s="32"/>
-      <c r="Q39" s="32"/>
-      <c r="R39" s="33"/>
+      <c r="C39" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="36"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="36"/>
+      <c r="M39" s="36"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="P39" s="36"/>
+      <c r="Q39" s="36"/>
+      <c r="R39" s="37"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="A40" s="16">
         <v>608</v>
       </c>
-      <c r="B40" s="26" t="str">
+      <c r="B40" s="13" t="str">
         <f t="shared" si="2"/>
         <v>0x00000260</v>
       </c>
-      <c r="C40" s="31" t="s">
+      <c r="C40" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="H40" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="35" t="s">
+      <c r="I40" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="H40" s="36" t="s">
+      <c r="J40" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="I40" s="36" t="s">
+      <c r="K40" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="J40" s="36" t="s">
+      <c r="L40" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="K40" s="36" t="s">
+      <c r="M40" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="L40" s="36" t="s">
+      <c r="N40" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="M40" s="36" t="s">
+      <c r="O40" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="N40" s="36" t="s">
+      <c r="P40" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="O40" s="36" t="s">
+      <c r="Q40" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="P40" s="36" t="s">
+      <c r="R40" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="Q40" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="R40" s="36" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="A41" s="16">
         <v>624</v>
       </c>
-      <c r="B41" s="26" t="str">
+      <c r="B41" s="13" t="str">
         <f t="shared" si="2"/>
         <v>0x00000270</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E41" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="36" t="s">
+      <c r="F41" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="E41" s="36" t="s">
+      <c r="G41" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="F41" s="36" t="s">
+      <c r="H41" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="G41" s="36" t="s">
+      <c r="I41" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="H41" s="36" t="s">
+      <c r="J41" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="I41" s="36" t="s">
+      <c r="K41" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="J41" s="36" t="s">
+      <c r="L41" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="K41" s="36" t="s">
+      <c r="M41" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="L41" s="37" t="s">
+      <c r="N41" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="M41" s="37" t="s">
+      <c r="O41" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="N41" s="37" t="s">
+      <c r="P41" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="O41" s="37" t="s">
+      <c r="Q41" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="P41" s="37" t="s">
+      <c r="R41" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="Q41" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="R41" s="37" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="A42" s="16">
         <v>640</v>
       </c>
-      <c r="B42" s="26" t="str">
+      <c r="B42" s="13" t="str">
         <f t="shared" si="2"/>
         <v>0x00000280</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E42" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="D42" s="37" t="s">
+      <c r="F42" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="E42" s="37" t="s">
+      <c r="G42" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="F42" s="37" t="s">
+      <c r="H42" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="G42" s="37" t="s">
+      <c r="I42" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="H42" s="37" t="s">
+      <c r="J42" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="I42" s="37" t="s">
+      <c r="K42" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="J42" s="37" t="s">
+      <c r="L42" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="K42" s="37" t="s">
+      <c r="M42" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="L42" s="37" t="s">
+      <c r="N42" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="M42" s="37" t="s">
+      <c r="O42" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="N42" s="37" t="s">
+      <c r="P42" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="O42" s="37" t="s">
+      <c r="Q42" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="R42" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="P42" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q42" s="50"/>
-      <c r="R42" s="35" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="A43" s="16">
         <v>656</v>
       </c>
-      <c r="B43" s="26" t="str">
+      <c r="B43" s="13" t="str">
         <f t="shared" si="2"/>
         <v>0x00000290</v>
       </c>
-      <c r="C43" s="47" t="s">
+      <c r="C43" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="47" t="s">
-        <v>229</v>
-      </c>
-      <c r="H43" s="48"/>
-      <c r="I43" s="48"/>
-      <c r="J43" s="49"/>
-      <c r="K43" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="L43" s="48"/>
-      <c r="M43" s="48"/>
-      <c r="N43" s="49"/>
-      <c r="O43" s="47" t="s">
-        <v>225</v>
-      </c>
-      <c r="P43" s="48"/>
-      <c r="Q43" s="48"/>
-      <c r="R43" s="49"/>
-      <c r="T43" t="s">
-        <v>249</v>
+      <c r="L43" s="39"/>
+      <c r="M43" s="39"/>
+      <c r="N43" s="40"/>
+      <c r="O43" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="P43" s="39"/>
+      <c r="Q43" s="39"/>
+      <c r="R43" s="40"/>
+      <c r="T43" s="16" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A44">
+      <c r="A44" s="16">
         <v>672</v>
       </c>
-      <c r="B44" s="26" t="str">
+      <c r="B44" s="13" t="str">
         <f>"0x"&amp;DEC2HEX(A44,8)</f>
         <v>0x000002A0</v>
       </c>
-      <c r="C44" s="47" t="s">
-        <v>226</v>
-      </c>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="49"/>
-      <c r="K44" s="47" t="s">
-        <v>231</v>
-      </c>
-      <c r="L44" s="48"/>
-      <c r="M44" s="48"/>
-      <c r="N44" s="49"/>
-      <c r="O44" s="47" t="s">
-        <v>232</v>
-      </c>
-      <c r="P44" s="48"/>
-      <c r="Q44" s="48"/>
-      <c r="R44" s="49"/>
+      <c r="C44" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="L44" s="39"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="40"/>
+      <c r="O44" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="P44" s="39"/>
+      <c r="Q44" s="39"/>
+      <c r="R44" s="40"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="A45" s="16">
         <v>688</v>
       </c>
-      <c r="B45" s="26" t="str">
+      <c r="B45" s="13" t="str">
         <f>"0x"&amp;DEC2HEX(A45,8)</f>
         <v>0x000002B0</v>
       </c>
-      <c r="C45" s="47" t="s">
+      <c r="C45" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="H45" s="39"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="D45" s="48"/>
-      <c r="E45" s="48"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="47" t="s">
+      <c r="L45" s="39"/>
+      <c r="M45" s="39"/>
+      <c r="N45" s="40"/>
+      <c r="O45" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="H45" s="48"/>
-      <c r="I45" s="48"/>
-      <c r="J45" s="49"/>
-      <c r="K45" s="47" t="s">
-        <v>235</v>
-      </c>
-      <c r="L45" s="48"/>
-      <c r="M45" s="48"/>
-      <c r="N45" s="49"/>
-      <c r="O45" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="P45" s="48"/>
-      <c r="Q45" s="48"/>
-      <c r="R45" s="49"/>
+      <c r="P45" s="39"/>
+      <c r="Q45" s="39"/>
+      <c r="R45" s="40"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="A46" s="16">
         <v>704</v>
       </c>
-      <c r="B46" s="26" t="str">
+      <c r="B46" s="13" t="str">
         <f t="shared" ref="B46" si="3">"0x"&amp;DEC2HEX(A46,8)</f>
         <v>0x000002C0</v>
       </c>
-      <c r="C46" s="47" t="s">
+      <c r="C46" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="H46" s="39"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="47" t="s">
+      <c r="L46" s="39"/>
+      <c r="M46" s="39"/>
+      <c r="N46" s="40"/>
+      <c r="O46" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="H46" s="48"/>
-      <c r="I46" s="48"/>
-      <c r="J46" s="49"/>
-      <c r="K46" s="47" t="s">
-        <v>239</v>
-      </c>
-      <c r="L46" s="48"/>
-      <c r="M46" s="48"/>
-      <c r="N46" s="49"/>
-      <c r="O46" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="P46" s="48"/>
-      <c r="Q46" s="48"/>
-      <c r="R46" s="49"/>
+      <c r="P46" s="39"/>
+      <c r="Q46" s="39"/>
+      <c r="R46" s="40"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A47">
+      <c r="A47" s="16">
         <v>720</v>
       </c>
-      <c r="B47" s="26" t="str">
+      <c r="B47" s="13" t="str">
         <f>"0x"&amp;DEC2HEX(A47,8)</f>
         <v>0x000002D0</v>
       </c>
-      <c r="C47" s="47" t="s">
+      <c r="C47" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="H47" s="39"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="47" t="s">
+      <c r="L47" s="39"/>
+      <c r="M47" s="39"/>
+      <c r="N47" s="40"/>
+      <c r="O47" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="H47" s="48"/>
-      <c r="I47" s="48"/>
-      <c r="J47" s="49"/>
-      <c r="K47" s="47" t="s">
-        <v>243</v>
-      </c>
-      <c r="L47" s="48"/>
-      <c r="M47" s="48"/>
-      <c r="N47" s="49"/>
-      <c r="O47" s="47" t="s">
-        <v>244</v>
-      </c>
-      <c r="P47" s="48"/>
-      <c r="Q47" s="48"/>
-      <c r="R47" s="49"/>
+      <c r="P47" s="39"/>
+      <c r="Q47" s="39"/>
+      <c r="R47" s="40"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A48">
+      <c r="A48" s="16">
         <v>736</v>
       </c>
-      <c r="B48" s="26" t="str">
+      <c r="B48" s="13" t="str">
         <f>"0x"&amp;DEC2HEX(A48,8)</f>
         <v>0x000002E0</v>
       </c>
-      <c r="C48" s="47" t="s">
+      <c r="C48" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="H48" s="39"/>
+      <c r="I48" s="39"/>
+      <c r="J48" s="40"/>
+      <c r="K48" s="38" t="s">
         <v>245</v>
       </c>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="47" t="s">
+      <c r="L48" s="39"/>
+      <c r="M48" s="39"/>
+      <c r="N48" s="40"/>
+      <c r="O48" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="H48" s="48"/>
-      <c r="I48" s="48"/>
-      <c r="J48" s="49"/>
-      <c r="K48" s="47" t="s">
-        <v>247</v>
-      </c>
-      <c r="L48" s="48"/>
-      <c r="M48" s="48"/>
-      <c r="N48" s="49"/>
-      <c r="O48" s="47" t="s">
-        <v>248</v>
-      </c>
-      <c r="P48" s="48"/>
-      <c r="Q48" s="48"/>
-      <c r="R48" s="49"/>
+      <c r="P48" s="39"/>
+      <c r="Q48" s="39"/>
+      <c r="R48" s="40"/>
     </row>
     <row r="51" spans="19:20" x14ac:dyDescent="0.3">
-      <c r="S51" s="20"/>
-      <c r="T51" t="s">
-        <v>252</v>
+      <c r="S51" s="19"/>
+      <c r="T51" s="16" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3350,42 +3501,42 @@
   <sheetData>
     <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="17" t="s">
+      <c r="B1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="21" t="s">
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="1">

</xml_diff>

<commit_message>
kept implementing ROM file writing
</commit_message>
<xml_diff>
--- a/tool-defs/ndi_rom_format.xlsx
+++ b/tool-defs/ndi_rom_format.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="260">
   <si>
     <t>YEAR</t>
   </si>
@@ -802,6 +802,9 @@
   </si>
   <si>
     <t>Not sure what 0x20 and 0x41 represent…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marker Type: 0x11 = 880 Active Ceramic; 0x12 = 930; 0x10 = NDI Legacy; 0x29 = Passive Marker, Sphere; 0x31 = Passive Marker, Disk </t>
   </si>
 </sst>
 </file>
@@ -916,7 +919,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -944,6 +947,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1070,9 +1079,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1097,18 +1103,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1118,39 +1112,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1158,6 +1119,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1192,6 +1156,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1480,1894 +1489,1927 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21:N21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="0" style="16" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="8.88671875" style="26"/>
-    <col min="12" max="12" width="10.77734375" style="26" customWidth="1"/>
-    <col min="13" max="14" width="8.88671875" style="26"/>
-    <col min="15" max="15" width="10.21875" style="26" customWidth="1"/>
-    <col min="16" max="17" width="8.88671875" style="26"/>
-    <col min="18" max="18" width="10.33203125" style="26" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" style="16"/>
-    <col min="20" max="20" width="114.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.88671875" style="16"/>
+    <col min="1" max="1" width="0" style="15" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="8.88671875" style="21"/>
+    <col min="12" max="12" width="10.77734375" style="21" customWidth="1"/>
+    <col min="13" max="14" width="8.88671875" style="21"/>
+    <col min="15" max="15" width="10.21875" style="21" customWidth="1"/>
+    <col min="16" max="17" width="8.88671875" style="21"/>
+    <col min="18" max="18" width="10.33203125" style="21" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" style="15"/>
+    <col min="20" max="20" width="114.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13">
-        <v>0</v>
-      </c>
-      <c r="D1" s="13">
-        <v>1</v>
-      </c>
-      <c r="E1" s="13">
+    <row r="1" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12">
+        <v>0</v>
+      </c>
+      <c r="D1" s="12">
+        <v>1</v>
+      </c>
+      <c r="E1" s="12">
         <v>2</v>
       </c>
-      <c r="F1" s="13">
+      <c r="F1" s="12">
         <v>3</v>
       </c>
-      <c r="G1" s="13">
+      <c r="G1" s="12">
         <v>4</v>
       </c>
-      <c r="H1" s="13">
+      <c r="H1" s="12">
         <v>5</v>
       </c>
-      <c r="I1" s="13">
+      <c r="I1" s="12">
         <v>6</v>
       </c>
-      <c r="J1" s="13">
+      <c r="J1" s="12">
         <v>7</v>
       </c>
-      <c r="K1" s="13">
+      <c r="K1" s="12">
         <v>8</v>
       </c>
-      <c r="L1" s="13">
+      <c r="L1" s="12">
         <v>9</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="T1" s="14" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="16">
-        <v>0</v>
-      </c>
-      <c r="B2" s="13" t="str">
+      <c r="A2" s="15">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12" t="str">
         <f>"0x"&amp;DEC2HEX(A2,8)</f>
         <v>0x00000000</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="25" t="s">
         <v>254</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="17" t="s">
+      <c r="H2" s="25"/>
+      <c r="I2" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="R2" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="T2" s="15" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <v>16</v>
       </c>
-      <c r="B3" s="13" t="str">
+      <c r="B3" s="12" t="str">
         <f>"0x"&amp;DEC2HEX(A3,8)</f>
         <v>0x00000010</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="11" t="s">
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q3" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="R3" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="T3" s="15" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
+      <c r="A4" s="15">
         <v>32</v>
       </c>
-      <c r="B4" s="13" t="str">
+      <c r="B4" s="12" t="str">
         <f t="shared" ref="B4:B21" si="0">"0x"&amp;DEC2HEX(A4,8)</f>
         <v>0x00000020</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="37" t="s">
         <v>255</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27" t="s">
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27" t="s">
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="T4" s="16" t="s">
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="T4" s="15" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
+      <c r="A5" s="15">
         <v>48</v>
       </c>
-      <c r="B5" s="13" t="str">
+      <c r="B5" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x00000030</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="17" t="s">
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="N5" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="O5" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="P5" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="Q5" s="17" t="s">
+      <c r="Q5" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="R5" s="17" t="s">
+      <c r="R5" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="T5" s="16" t="s">
+      <c r="T5" s="15" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>64</v>
       </c>
-      <c r="B6" s="13" t="str">
+      <c r="B6" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x00000040</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="K6" s="28" t="s">
+      <c r="K6" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="28" t="s">
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="30"/>
-      <c r="T6" s="16" t="s">
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="41"/>
+      <c r="T6" s="15" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <v>80</v>
       </c>
-      <c r="B7" s="13" t="str">
+      <c r="B7" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x00000050</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="28" t="s">
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="28" t="s">
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="28" t="s">
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="39" t="s">
         <v>194</v>
       </c>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="30"/>
-      <c r="T7" s="16" t="s">
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="41"/>
+      <c r="T7" s="15" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="16">
+      <c r="A8" s="15">
         <v>96</v>
       </c>
-      <c r="B8" s="13" t="str">
+      <c r="B8" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x00000060</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="28" t="s">
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="28" t="s">
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="28" t="s">
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="30"/>
-      <c r="T8" s="16" t="s">
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="41"/>
+      <c r="T8" s="15" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <v>112</v>
       </c>
-      <c r="B9" s="13" t="str">
+      <c r="B9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x00000070</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="28" t="s">
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="39" t="s">
         <v>196</v>
       </c>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="28" t="s">
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="28" t="s">
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="30"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="41"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <v>128</v>
       </c>
-      <c r="B10" s="13" t="str">
+      <c r="B10" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x00000080</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="28" t="s">
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="28" t="s">
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="28" t="s">
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="30"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="41"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="16">
+      <c r="A11" s="15">
         <v>144</v>
       </c>
-      <c r="B11" s="13" t="str">
+      <c r="B11" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x00000090</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="28" t="s">
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="28" t="s">
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="28" t="s">
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="30"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="41"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <v>160</v>
       </c>
-      <c r="B12" s="13" t="str">
+      <c r="B12" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x000000A0</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="28" t="s">
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="28" t="s">
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="28" t="s">
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="30"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="41"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="16">
+      <c r="A13" s="15">
         <v>176</v>
       </c>
-      <c r="B13" s="13" t="str">
+      <c r="B13" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x000000B0</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="39" t="s">
         <v>201</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="28" t="s">
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="28" t="s">
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="28" t="s">
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="30"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="41"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="16">
+      <c r="A14" s="15">
         <v>192</v>
       </c>
-      <c r="B14" s="13" t="str">
+      <c r="B14" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x000000C0</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="28" t="s">
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="28" t="s">
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="28" t="s">
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="30"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="41"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="16">
+      <c r="A15" s="15">
         <v>208</v>
       </c>
-      <c r="B15" s="13" t="str">
+      <c r="B15" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x000000D0</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="28" t="s">
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="28" t="s">
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="28" t="s">
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="29"/>
-      <c r="R15" s="30"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="41"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="16">
+      <c r="A16" s="15">
         <v>224</v>
       </c>
-      <c r="B16" s="13" t="str">
+      <c r="B16" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x000000E0</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="39" t="s">
         <v>205</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="28" t="s">
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="28" t="s">
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="28" t="s">
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="30"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="41"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="16">
+      <c r="A17" s="15">
         <v>240</v>
       </c>
-      <c r="B17" s="13" t="str">
+      <c r="B17" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x000000F0</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="28" t="s">
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="39" t="s">
         <v>187</v>
       </c>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="28" t="s">
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="39" t="s">
         <v>207</v>
       </c>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="28" t="s">
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="30"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="41"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="16">
+      <c r="A18" s="15">
         <v>256</v>
       </c>
-      <c r="B18" s="13" t="str">
+      <c r="B18" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x00000100</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="39" t="s">
         <v>188</v>
       </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="28" t="s">
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="39" t="s">
         <v>208</v>
       </c>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="28" t="s">
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="28" t="s">
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="30"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="41"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="16">
+      <c r="A19" s="15">
         <v>272</v>
       </c>
-      <c r="B19" s="13" t="str">
+      <c r="B19" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x00000110</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="39" t="s">
         <v>209</v>
       </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="28" t="s">
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="28" t="s">
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="39" t="s">
         <v>190</v>
       </c>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="28" t="s">
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29"/>
-      <c r="R19" s="30"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="41"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="16">
+      <c r="A20" s="15">
         <v>288</v>
       </c>
-      <c r="B20" s="13" t="str">
+      <c r="B20" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x00000120</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="28" t="s">
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="28" t="s">
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="39" t="s">
         <v>211</v>
       </c>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="28" t="s">
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="30"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="41"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="16">
+      <c r="A21" s="15">
         <v>304</v>
       </c>
-      <c r="B21" s="13" t="str">
+      <c r="B21" s="12" t="str">
         <f t="shared" si="0"/>
         <v>0x00000130</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="28" t="s">
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="39" t="s">
         <v>212</v>
       </c>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="32" t="s">
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="32" t="s">
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="34"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="44"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="16">
+      <c r="A22" s="15">
         <v>320</v>
       </c>
-      <c r="B22" s="13" t="str">
+      <c r="B22" s="12" t="str">
         <f>"0x"&amp;DEC2HEX(A22,8)</f>
         <v>0x00000140</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="32" t="s">
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="32" t="s">
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="32" t="s">
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="34"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="44"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="16">
+      <c r="A23" s="15">
         <v>336</v>
       </c>
-      <c r="B23" s="13" t="str">
+      <c r="B23" s="12" t="str">
         <f>"0x"&amp;DEC2HEX(A23,8)</f>
         <v>0x00000150</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="32" t="s">
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="32" t="s">
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="32" t="s">
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
-      <c r="R23" s="34"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="44"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="16">
+      <c r="A24" s="15">
         <v>352</v>
       </c>
-      <c r="B24" s="13" t="str">
+      <c r="B24" s="12" t="str">
         <f t="shared" ref="B24:B31" si="1">"0x"&amp;DEC2HEX(A24,8)</f>
         <v>0x00000160</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="32" t="s">
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="32" t="s">
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="32" t="s">
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="34"/>
+      <c r="P24" s="43"/>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="44"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="16">
+      <c r="A25" s="15">
         <v>368</v>
       </c>
-      <c r="B25" s="13" t="str">
+      <c r="B25" s="12" t="str">
         <f t="shared" si="1"/>
         <v>0x00000170</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="32" t="s">
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="32" t="s">
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="32" t="s">
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="P25" s="33"/>
-      <c r="Q25" s="33"/>
-      <c r="R25" s="34"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="44"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="16">
+      <c r="A26" s="15">
         <v>384</v>
       </c>
-      <c r="B26" s="13" t="str">
+      <c r="B26" s="12" t="str">
         <f t="shared" si="1"/>
         <v>0x00000180</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="32" t="s">
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="32" t="s">
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="32" t="s">
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="P26" s="33"/>
-      <c r="Q26" s="33"/>
-      <c r="R26" s="34"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="44"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="16">
+      <c r="A27" s="15">
         <v>400</v>
       </c>
-      <c r="B27" s="13" t="str">
+      <c r="B27" s="12" t="str">
         <f t="shared" si="1"/>
         <v>0x00000190</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="32" t="s">
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="32" t="s">
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="34"/>
-      <c r="O27" s="32" t="s">
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="34"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="44"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="16">
+      <c r="A28" s="15">
         <v>416</v>
       </c>
-      <c r="B28" s="13" t="str">
+      <c r="B28" s="12" t="str">
         <f t="shared" si="1"/>
         <v>0x000001A0</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="32" t="s">
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="32" t="s">
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="32" t="s">
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="P28" s="33"/>
-      <c r="Q28" s="33"/>
-      <c r="R28" s="34"/>
+      <c r="P28" s="43"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="44"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="16">
+      <c r="A29" s="15">
         <v>432</v>
       </c>
-      <c r="B29" s="13" t="str">
+      <c r="B29" s="12" t="str">
         <f t="shared" si="1"/>
         <v>0x000001B0</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="32" t="s">
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="32" t="s">
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="34"/>
-      <c r="O29" s="32" t="s">
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="P29" s="33"/>
-      <c r="Q29" s="33"/>
-      <c r="R29" s="34"/>
+      <c r="P29" s="43"/>
+      <c r="Q29" s="43"/>
+      <c r="R29" s="44"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="16">
+      <c r="A30" s="15">
         <v>448</v>
       </c>
-      <c r="B30" s="13" t="str">
+      <c r="B30" s="12" t="str">
         <f t="shared" si="1"/>
         <v>0x000001C0</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="32" t="s">
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="32" t="s">
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="34"/>
-      <c r="O30" s="32" t="s">
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="P30" s="33"/>
-      <c r="Q30" s="33"/>
-      <c r="R30" s="34"/>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="44"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="16">
+      <c r="A31" s="15">
         <v>464</v>
       </c>
-      <c r="B31" s="13" t="str">
+      <c r="B31" s="12" t="str">
         <f t="shared" si="1"/>
         <v>0x000001D0</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="32" t="s">
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="32" t="s">
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="34"/>
-      <c r="O31" s="32" t="s">
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="44"/>
+      <c r="O31" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="33"/>
-      <c r="R31" s="34"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="44"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="16">
+      <c r="A32" s="15">
         <v>480</v>
       </c>
-      <c r="B32" s="13" t="str">
+      <c r="B32" s="12" t="str">
         <f>"0x"&amp;DEC2HEX(A32,8)</f>
         <v>0x000001E0</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="32" t="s">
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="32" t="s">
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="32" t="s">
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="P32" s="33"/>
-      <c r="Q32" s="33"/>
-      <c r="R32" s="34"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="44"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A33" s="16">
+      <c r="A33" s="15">
         <v>496</v>
       </c>
-      <c r="B33" s="13" t="str">
+      <c r="B33" s="12" t="str">
         <f>"0x"&amp;DEC2HEX(A33,8)</f>
         <v>0x000001F0</v>
       </c>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="32" t="s">
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="32" t="s">
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="34"/>
-      <c r="O33" s="32" t="s">
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="44"/>
+      <c r="O33" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="P33" s="33"/>
-      <c r="Q33" s="33"/>
-      <c r="R33" s="34"/>
+      <c r="P33" s="43"/>
+      <c r="Q33" s="43"/>
+      <c r="R33" s="44"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A34" s="16">
+      <c r="A34" s="15">
         <v>512</v>
       </c>
-      <c r="B34" s="13" t="str">
+      <c r="B34" s="12" t="str">
         <f t="shared" ref="B34:B43" si="2">"0x"&amp;DEC2HEX(A34,8)</f>
         <v>0x00000200</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="32" t="s">
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="32" t="s">
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
-      <c r="N34" s="34"/>
-      <c r="O34" s="32" t="s">
+      <c r="L34" s="43"/>
+      <c r="M34" s="43"/>
+      <c r="N34" s="44"/>
+      <c r="O34" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="P34" s="33"/>
-      <c r="Q34" s="33"/>
-      <c r="R34" s="34"/>
+      <c r="P34" s="43"/>
+      <c r="Q34" s="43"/>
+      <c r="R34" s="44"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A35" s="16">
+      <c r="A35" s="15">
         <v>528</v>
       </c>
-      <c r="B35" s="13" t="str">
+      <c r="B35" s="12" t="str">
         <f t="shared" si="2"/>
         <v>0x00000210</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="C35" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="32" t="s">
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="32" t="s">
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="L35" s="33"/>
-      <c r="M35" s="33"/>
-      <c r="N35" s="34"/>
-      <c r="O35" s="32" t="s">
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="44"/>
+      <c r="O35" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="P35" s="33"/>
-      <c r="Q35" s="33"/>
-      <c r="R35" s="34"/>
+      <c r="P35" s="43"/>
+      <c r="Q35" s="43"/>
+      <c r="R35" s="44"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A36" s="16">
+      <c r="A36" s="15">
         <v>544</v>
       </c>
-      <c r="B36" s="13" t="str">
+      <c r="B36" s="12" t="str">
         <f t="shared" si="2"/>
         <v>0x00000220</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="32" t="s">
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="H36" s="33"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="20" t="s">
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="L36" s="20" t="s">
+      <c r="L36" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="M36" s="20" t="s">
+      <c r="M36" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="N36" s="20" t="s">
+      <c r="N36" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="O36" s="20" t="s">
+      <c r="O36" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="P36" s="20" t="s">
+      <c r="P36" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="Q36" s="20" t="s">
+      <c r="Q36" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="R36" s="20" t="s">
+      <c r="R36" s="45" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A37" s="16">
+      <c r="A37" s="15">
         <v>560</v>
       </c>
-      <c r="B37" s="13" t="str">
+      <c r="B37" s="12" t="str">
         <f t="shared" si="2"/>
         <v>0x00000230</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="E37" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="F37" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="G37" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="H37" s="20" t="s">
+      <c r="H37" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="I37" s="20" t="s">
+      <c r="I37" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="J37" s="20" t="s">
+      <c r="J37" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="K37" s="20" t="s">
+      <c r="K37" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="L37" s="20" t="s">
+      <c r="L37" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="M37" s="20" t="s">
+      <c r="M37" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="N37" s="20" t="s">
+      <c r="N37" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="O37" s="21" t="s">
+      <c r="O37" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="P37" s="21" t="s">
+      <c r="P37" s="46" t="s">
         <v>215</v>
       </c>
-      <c r="Q37" s="21" t="s">
+      <c r="Q37" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="R37" s="21" t="s">
+      <c r="R37" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="T37" s="16" t="s">
+      <c r="T37" s="15" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A38" s="16">
+      <c r="A38" s="15">
         <v>576</v>
       </c>
-      <c r="B38" s="13" t="str">
+      <c r="B38" s="12" t="str">
         <f t="shared" si="2"/>
         <v>0x00000240</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="47" t="s">
         <v>218</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="47" t="s">
         <v>219</v>
       </c>
-      <c r="E38" s="22" t="s">
+      <c r="E38" s="47" t="s">
         <v>220</v>
       </c>
-      <c r="F38" s="22" t="s">
+      <c r="F38" s="47" t="s">
         <v>221</v>
       </c>
-      <c r="G38" s="35" t="s">
+      <c r="G38" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="36"/>
-      <c r="N38" s="36"/>
-      <c r="O38" s="36"/>
-      <c r="P38" s="36"/>
-      <c r="Q38" s="36"/>
-      <c r="R38" s="37"/>
-      <c r="T38" s="16" t="s">
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="49"/>
+      <c r="O38" s="49"/>
+      <c r="P38" s="49"/>
+      <c r="Q38" s="49"/>
+      <c r="R38" s="50"/>
+      <c r="T38" s="15" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A39" s="16">
+      <c r="A39" s="15">
         <v>592</v>
       </c>
-      <c r="B39" s="13" t="str">
+      <c r="B39" s="12" t="str">
         <f t="shared" si="2"/>
         <v>0x00000250</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="P39" s="36"/>
-      <c r="Q39" s="36"/>
-      <c r="R39" s="37"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="49"/>
+      <c r="P39" s="49"/>
+      <c r="Q39" s="49"/>
+      <c r="R39" s="50"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A40" s="16">
+      <c r="A40" s="15">
         <v>608</v>
       </c>
-      <c r="B40" s="13" t="str">
+      <c r="B40" s="12" t="str">
         <f t="shared" si="2"/>
         <v>0x00000260</v>
       </c>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="23" t="s">
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="H40" s="24" t="s">
+      <c r="H40" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="I40" s="24" t="s">
+      <c r="I40" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="J40" s="24" t="s">
+      <c r="J40" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="K40" s="24" t="s">
+      <c r="K40" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="L40" s="24" t="s">
+      <c r="L40" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="M40" s="24" t="s">
+      <c r="M40" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="N40" s="24" t="s">
+      <c r="N40" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="O40" s="24" t="s">
+      <c r="O40" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="P40" s="24" t="s">
+      <c r="P40" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="Q40" s="24" t="s">
+      <c r="Q40" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="R40" s="24" t="s">
+      <c r="R40" s="19" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A41" s="16">
+      <c r="A41" s="15">
         <v>624</v>
       </c>
-      <c r="B41" s="13" t="str">
+      <c r="B41" s="12" t="str">
         <f t="shared" si="2"/>
         <v>0x00000270</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D41" s="24" t="s">
+      <c r="D41" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="F41" s="24" t="s">
+      <c r="F41" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="G41" s="24" t="s">
+      <c r="G41" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="H41" s="24" t="s">
+      <c r="H41" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="I41" s="24" t="s">
+      <c r="I41" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="J41" s="24" t="s">
+      <c r="J41" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="K41" s="24" t="s">
+      <c r="K41" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="L41" s="25" t="s">
+      <c r="L41" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="M41" s="25" t="s">
+      <c r="M41" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="N41" s="25" t="s">
+      <c r="N41" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="O41" s="25" t="s">
+      <c r="O41" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="P41" s="25" t="s">
+      <c r="P41" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="Q41" s="25" t="s">
+      <c r="Q41" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="R41" s="25" t="s">
+      <c r="R41" s="20" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A42" s="16">
+      <c r="A42" s="15">
         <v>640</v>
       </c>
-      <c r="B42" s="13" t="str">
+      <c r="B42" s="12" t="str">
         <f t="shared" si="2"/>
         <v>0x00000280</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="D42" s="25" t="s">
+      <c r="D42" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="E42" s="25" t="s">
+      <c r="E42" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="F42" s="25" t="s">
+      <c r="F42" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="G42" s="25" t="s">
+      <c r="G42" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="I42" s="25" t="s">
+      <c r="I42" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="J42" s="25" t="s">
+      <c r="J42" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="K42" s="25" t="s">
+      <c r="K42" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="L42" s="25" t="s">
+      <c r="L42" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="M42" s="25" t="s">
+      <c r="M42" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="N42" s="25" t="s">
+      <c r="N42" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="O42" s="25" t="s">
+      <c r="O42" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="P42" s="23" t="s">
+      <c r="P42" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="Q42" s="17" t="s">
+      <c r="Q42" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="R42" s="23" t="s">
+      <c r="R42" s="51" t="s">
         <v>148</v>
       </c>
+      <c r="T42" s="15" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A43" s="16">
+      <c r="A43" s="15">
         <v>656</v>
       </c>
-      <c r="B43" s="13" t="str">
+      <c r="B43" s="12" t="str">
         <f t="shared" si="2"/>
         <v>0x00000290</v>
       </c>
-      <c r="C43" s="38" t="s">
+      <c r="C43" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="38" t="s">
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="38" t="s">
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="L43" s="39"/>
-      <c r="M43" s="39"/>
-      <c r="N43" s="40"/>
-      <c r="O43" s="38" t="s">
+      <c r="L43" s="23"/>
+      <c r="M43" s="23"/>
+      <c r="N43" s="24"/>
+      <c r="O43" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="P43" s="39"/>
-      <c r="Q43" s="39"/>
-      <c r="R43" s="40"/>
-      <c r="T43" s="16" t="s">
+      <c r="P43" s="23"/>
+      <c r="Q43" s="23"/>
+      <c r="R43" s="24"/>
+      <c r="T43" s="15" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A44" s="16">
+      <c r="A44" s="15">
         <v>672</v>
       </c>
-      <c r="B44" s="13" t="str">
+      <c r="B44" s="12" t="str">
         <f>"0x"&amp;DEC2HEX(A44,8)</f>
         <v>0x000002A0</v>
       </c>
-      <c r="C44" s="38" t="s">
+      <c r="C44" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="38" t="s">
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="40"/>
-      <c r="K44" s="38" t="s">
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="40"/>
-      <c r="O44" s="38" t="s">
+      <c r="L44" s="23"/>
+      <c r="M44" s="23"/>
+      <c r="N44" s="24"/>
+      <c r="O44" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="P44" s="39"/>
-      <c r="Q44" s="39"/>
-      <c r="R44" s="40"/>
+      <c r="P44" s="23"/>
+      <c r="Q44" s="23"/>
+      <c r="R44" s="24"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A45" s="16">
+      <c r="A45" s="15">
         <v>688</v>
       </c>
-      <c r="B45" s="13" t="str">
+      <c r="B45" s="12" t="str">
         <f>"0x"&amp;DEC2HEX(A45,8)</f>
         <v>0x000002B0</v>
       </c>
-      <c r="C45" s="38" t="s">
+      <c r="C45" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="38" t="s">
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="40"/>
-      <c r="K45" s="38" t="s">
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="L45" s="39"/>
-      <c r="M45" s="39"/>
-      <c r="N45" s="40"/>
-      <c r="O45" s="38" t="s">
+      <c r="L45" s="23"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="24"/>
+      <c r="O45" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="P45" s="39"/>
-      <c r="Q45" s="39"/>
-      <c r="R45" s="40"/>
+      <c r="P45" s="23"/>
+      <c r="Q45" s="23"/>
+      <c r="R45" s="24"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A46" s="16">
+      <c r="A46" s="15">
         <v>704</v>
       </c>
-      <c r="B46" s="13" t="str">
+      <c r="B46" s="12" t="str">
         <f t="shared" ref="B46" si="3">"0x"&amp;DEC2HEX(A46,8)</f>
         <v>0x000002C0</v>
       </c>
-      <c r="C46" s="38" t="s">
+      <c r="C46" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="38" t="s">
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="H46" s="39"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="40"/>
-      <c r="K46" s="38" t="s">
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="L46" s="39"/>
-      <c r="M46" s="39"/>
-      <c r="N46" s="40"/>
-      <c r="O46" s="38" t="s">
+      <c r="L46" s="23"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="P46" s="39"/>
-      <c r="Q46" s="39"/>
-      <c r="R46" s="40"/>
+      <c r="P46" s="23"/>
+      <c r="Q46" s="23"/>
+      <c r="R46" s="24"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A47" s="16">
+      <c r="A47" s="15">
         <v>720</v>
       </c>
-      <c r="B47" s="13" t="str">
+      <c r="B47" s="12" t="str">
         <f>"0x"&amp;DEC2HEX(A47,8)</f>
         <v>0x000002D0</v>
       </c>
-      <c r="C47" s="38" t="s">
+      <c r="C47" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="38" t="s">
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="H47" s="39"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="40"/>
-      <c r="K47" s="38" t="s">
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="L47" s="39"/>
-      <c r="M47" s="39"/>
-      <c r="N47" s="40"/>
-      <c r="O47" s="38" t="s">
+      <c r="L47" s="23"/>
+      <c r="M47" s="23"/>
+      <c r="N47" s="24"/>
+      <c r="O47" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="P47" s="39"/>
-      <c r="Q47" s="39"/>
-      <c r="R47" s="40"/>
+      <c r="P47" s="23"/>
+      <c r="Q47" s="23"/>
+      <c r="R47" s="24"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A48" s="16">
+      <c r="A48" s="15">
         <v>736</v>
       </c>
-      <c r="B48" s="13" t="str">
+      <c r="B48" s="12" t="str">
         <f>"0x"&amp;DEC2HEX(A48,8)</f>
         <v>0x000002E0</v>
       </c>
-      <c r="C48" s="38" t="s">
+      <c r="C48" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="38" t="s">
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="H48" s="39"/>
-      <c r="I48" s="39"/>
-      <c r="J48" s="40"/>
-      <c r="K48" s="38" t="s">
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="24"/>
+      <c r="K48" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="L48" s="39"/>
-      <c r="M48" s="39"/>
-      <c r="N48" s="40"/>
-      <c r="O48" s="38" t="s">
+      <c r="L48" s="23"/>
+      <c r="M48" s="23"/>
+      <c r="N48" s="24"/>
+      <c r="O48" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="P48" s="39"/>
-      <c r="Q48" s="39"/>
-      <c r="R48" s="40"/>
+      <c r="P48" s="23"/>
+      <c r="Q48" s="23"/>
+      <c r="R48" s="24"/>
     </row>
     <row r="51" spans="19:20" x14ac:dyDescent="0.3">
-      <c r="S51" s="19"/>
-      <c r="T51" s="16" t="s">
+      <c r="S51" s="18"/>
+      <c r="T51" s="15" t="s">
         <v>250</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="154">
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="O47:R47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="G48:J48"/>
-    <mergeCell ref="K48:N48"/>
-    <mergeCell ref="O48:R48"/>
-    <mergeCell ref="O44:R44"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="G45:J45"/>
-    <mergeCell ref="K45:N45"/>
-    <mergeCell ref="O45:R45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="G46:J46"/>
-    <mergeCell ref="K46:N46"/>
-    <mergeCell ref="O46:R46"/>
-    <mergeCell ref="G38:R38"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="C39:R39"/>
-    <mergeCell ref="O43:R43"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="G43:J43"/>
-    <mergeCell ref="K43:N43"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="O7:R7"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="O10:R10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="O11:R11"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="O8:R8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="O9:R9"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="O15:R15"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="O12:R12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="O13:R13"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="O16:R16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="O17:R17"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="O19:R19"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="O26:R26"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="O27:R27"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="O22:R22"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="O24:R24"/>
     <mergeCell ref="K34:N34"/>
     <mergeCell ref="O34:R34"/>
     <mergeCell ref="K35:N35"/>
@@ -3392,85 +3434,57 @@
     <mergeCell ref="O30:R30"/>
     <mergeCell ref="K25:N25"/>
     <mergeCell ref="O25:R25"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="O26:R26"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="O27:R27"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="O22:R22"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="O24:R24"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="O19:R19"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="O16:R16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="O17:R17"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="O14:R14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="O15:R15"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="O12:R12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="O13:R13"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="O10:R10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="O11:R11"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="O8:R8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="O9:R9"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="O7:R7"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="G38:R38"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C39:R39"/>
+    <mergeCell ref="O43:R43"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="G43:J43"/>
+    <mergeCell ref="K43:N43"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="O47:R47"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="G48:J48"/>
+    <mergeCell ref="K48:N48"/>
+    <mergeCell ref="O48:R48"/>
+    <mergeCell ref="O44:R44"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="G45:J45"/>
+    <mergeCell ref="K45:N45"/>
+    <mergeCell ref="O45:R45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="G46:J46"/>
+    <mergeCell ref="K46:N46"/>
+    <mergeCell ref="O46:R46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3501,42 +3515,42 @@
   <sheetData>
     <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47" t="s">
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="50" t="s">
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="1">

</xml_diff>

<commit_message>
got tool definition ROM generation working
</commit_message>
<xml_diff>
--- a/tool-defs/ndi_rom_format.xlsx
+++ b/tool-defs/ndi_rom_format.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="261">
   <si>
     <t>YEAR</t>
   </si>
@@ -78,9 +78,6 @@
     <t>SeqNum</t>
   </si>
   <si>
-    <t>MAX ANGLE</t>
-  </si>
-  <si>
     <t># MARKERS</t>
   </si>
   <si>
@@ -477,9 +474,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>LITTLE ENDIAN format for values &gt; 1 char</t>
-  </si>
-  <si>
     <t>Checksum is simply sum of bytes 7 through end of file with 16bit overflow</t>
   </si>
   <si>
@@ -777,9 +771,6 @@
     <t>Subtype: 0x00 = Removable tip; 0x01= Fixed Tip; 0x02 = Undefined</t>
   </si>
   <si>
-    <t>Unknown: set to 0x00</t>
-  </si>
-  <si>
     <t>0x01</t>
   </si>
   <si>
@@ -789,9 +780,6 @@
     <t>Not sure what the 0x01 in byte 8 represents…</t>
   </si>
   <si>
-    <t>CHKSUM of 7:end</t>
-  </si>
-  <si>
     <t>MIN MKRS</t>
   </si>
   <si>
@@ -805,6 +793,21 @@
   </si>
   <si>
     <t xml:space="preserve">Marker Type: 0x11 = 880 Active Ceramic; 0x12 = 930; 0x10 = NDI Legacy; 0x29 = Passive Marker, Sphere; 0x31 = Passive Marker, Disk </t>
+  </si>
+  <si>
+    <t>Byte Addr.</t>
+  </si>
+  <si>
+    <t>MAX ANG</t>
+  </si>
+  <si>
+    <t>Unknown: set to value shown</t>
+  </si>
+  <si>
+    <t>LITTLE ENDIAN format for all values &gt; 1 char</t>
+  </si>
+  <si>
+    <t>CHKSUM of 7:752</t>
   </si>
 </sst>
 </file>
@@ -919,7 +922,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -941,12 +944,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1103,25 +1100,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1157,49 +1136,67 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1490,21 +1487,21 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0" style="15" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="8.88671875" style="21"/>
-    <col min="12" max="12" width="10.77734375" style="21" customWidth="1"/>
-    <col min="13" max="14" width="8.88671875" style="21"/>
-    <col min="15" max="15" width="10.21875" style="21" customWidth="1"/>
-    <col min="16" max="17" width="8.88671875" style="21"/>
-    <col min="18" max="18" width="10.33203125" style="21" customWidth="1"/>
+    <col min="3" max="11" width="8.88671875" style="19"/>
+    <col min="12" max="12" width="10.77734375" style="19" customWidth="1"/>
+    <col min="13" max="14" width="8.88671875" style="19"/>
+    <col min="15" max="15" width="10.21875" style="19" customWidth="1"/>
+    <col min="16" max="17" width="8.88671875" style="19"/>
+    <col min="18" max="18" width="10.33203125" style="19" customWidth="1"/>
     <col min="19" max="19" width="8.88671875" style="15"/>
     <col min="20" max="20" width="114.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="21" max="16384" width="8.88671875" style="15"/>
@@ -1512,7 +1509,9 @@
   <sheetData>
     <row r="1" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
-      <c r="B1" s="12"/>
+      <c r="B1" s="12" t="s">
+        <v>256</v>
+      </c>
       <c r="C1" s="12">
         <v>0</v>
       </c>
@@ -1562,7 +1561,7 @@
         <v>9</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -1573,54 +1572,54 @@
         <f>"0x"&amp;DEC2HEX(A2,8)</f>
         <v>0x00000000</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="31" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>254</v>
-      </c>
-      <c r="H2" s="25"/>
+        <v>249</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>260</v>
+      </c>
+      <c r="H2" s="51"/>
       <c r="I2" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="O2" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="O2" s="31" t="s">
         <v>12</v>
       </c>
       <c r="P2" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="Q2" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="R2" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="R2" s="31" t="s">
         <v>13</v>
       </c>
       <c r="T2" s="15" t="s">
-        <v>150</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -1631,50 +1630,50 @@
         <f>"0x"&amp;DEC2HEX(A3,8)</f>
         <v>0x00000010</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="G3" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="G3" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="37" t="s">
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="O3" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="O3" s="37" t="s">
-        <v>18</v>
-      </c>
       <c r="P3" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="R3" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="T3" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -1685,38 +1684,38 @@
         <f t="shared" ref="B4:B21" si="0">"0x"&amp;DEC2HEX(A4,8)</f>
         <v>0x00000020</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>255</v>
+      <c r="C4" s="31" t="s">
+        <v>251</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="G4" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38" t="s">
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
       <c r="T4" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -1727,50 +1726,50 @@
         <f t="shared" si="0"/>
         <v>0x00000030</v>
       </c>
-      <c r="C5" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="C5" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="Q5" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="R5" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="T5" s="15" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
@@ -1782,43 +1781,43 @@
         <v>0x00000040</v>
       </c>
       <c r="C6" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>256</v>
-      </c>
       <c r="F6" s="17" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="K6" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="39" t="s">
-        <v>173</v>
-      </c>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="41"/>
+        <v>249</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="35"/>
       <c r="T6" s="15" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
@@ -1829,32 +1828,32 @@
         <f t="shared" si="0"/>
         <v>0x00000050</v>
       </c>
-      <c r="C7" s="39" t="s">
-        <v>193</v>
-      </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="41"/>
+      <c r="C7" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="35"/>
       <c r="T7" s="15" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
@@ -1865,32 +1864,32 @@
         <f t="shared" si="0"/>
         <v>0x00000060</v>
       </c>
-      <c r="C8" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="39" t="s">
-        <v>195</v>
-      </c>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="41"/>
+      <c r="C8" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="35"/>
       <c r="T8" s="15" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -1901,30 +1900,30 @@
         <f t="shared" si="0"/>
         <v>0x00000070</v>
       </c>
-      <c r="C9" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="39" t="s">
-        <v>196</v>
-      </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="39" t="s">
-        <v>177</v>
-      </c>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="41"/>
+      <c r="C9" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="35"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
@@ -1934,30 +1933,30 @@
         <f t="shared" si="0"/>
         <v>0x00000080</v>
       </c>
-      <c r="C10" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="41"/>
+      <c r="C10" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="35"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
@@ -1967,30 +1966,30 @@
         <f t="shared" si="0"/>
         <v>0x00000090</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="39" t="s">
-        <v>179</v>
-      </c>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="41"/>
+      <c r="C11" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="35"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
@@ -2000,30 +1999,30 @@
         <f t="shared" si="0"/>
         <v>0x000000A0</v>
       </c>
-      <c r="C12" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="41"/>
+      <c r="C12" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="35"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
@@ -2033,30 +2032,30 @@
         <f t="shared" si="0"/>
         <v>0x000000B0</v>
       </c>
-      <c r="C13" s="39" t="s">
-        <v>201</v>
-      </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="39" t="s">
-        <v>182</v>
-      </c>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="39" t="s">
-        <v>202</v>
-      </c>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="41"/>
+      <c r="C13" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="35"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
@@ -2066,30 +2065,30 @@
         <f t="shared" si="0"/>
         <v>0x000000C0</v>
       </c>
-      <c r="C14" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="39" t="s">
-        <v>164</v>
-      </c>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="41"/>
+      <c r="C14" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="35"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
@@ -2099,30 +2098,30 @@
         <f t="shared" si="0"/>
         <v>0x000000D0</v>
       </c>
-      <c r="C15" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="39" t="s">
-        <v>204</v>
-      </c>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="41"/>
+      <c r="C15" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="35"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
@@ -2132,30 +2131,30 @@
         <f t="shared" si="0"/>
         <v>0x000000E0</v>
       </c>
-      <c r="C16" s="39" t="s">
-        <v>205</v>
-      </c>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="39" t="s">
-        <v>206</v>
-      </c>
-      <c r="P16" s="40"/>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="41"/>
+      <c r="C16" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="35"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
@@ -2165,30 +2164,30 @@
         <f t="shared" si="0"/>
         <v>0x000000F0</v>
       </c>
-      <c r="C17" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="39" t="s">
-        <v>207</v>
-      </c>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="39" t="s">
-        <v>168</v>
-      </c>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="41"/>
+      <c r="C17" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="35"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
@@ -2198,30 +2197,30 @@
         <f t="shared" si="0"/>
         <v>0x00000100</v>
       </c>
-      <c r="C18" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="39" t="s">
-        <v>208</v>
-      </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="39" t="s">
-        <v>169</v>
-      </c>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="39" t="s">
-        <v>189</v>
-      </c>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="41"/>
+      <c r="C18" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="35"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
@@ -2231,30 +2230,30 @@
         <f t="shared" si="0"/>
         <v>0x00000110</v>
       </c>
-      <c r="C19" s="39" t="s">
-        <v>209</v>
-      </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="39" t="s">
-        <v>210</v>
-      </c>
-      <c r="P19" s="40"/>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="41"/>
+      <c r="C19" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="35"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
@@ -2264,30 +2263,30 @@
         <f t="shared" si="0"/>
         <v>0x00000120</v>
       </c>
-      <c r="C20" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="39" t="s">
-        <v>211</v>
-      </c>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="P20" s="40"/>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="41"/>
+      <c r="C20" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="35"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
@@ -2297,30 +2296,30 @@
         <f t="shared" si="0"/>
         <v>0x00000130</v>
       </c>
-      <c r="C21" s="39" t="s">
-        <v>192</v>
-      </c>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="39" t="s">
-        <v>212</v>
-      </c>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="L21" s="43"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="43"/>
-      <c r="R21" s="44"/>
+      <c r="C21" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="38"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
@@ -2330,30 +2329,30 @@
         <f>"0x"&amp;DEC2HEX(A22,8)</f>
         <v>0x00000140</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="L22" s="43"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="P22" s="43"/>
-      <c r="Q22" s="43"/>
-      <c r="R22" s="44"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="38"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
@@ -2363,30 +2362,30 @@
         <f>"0x"&amp;DEC2HEX(A23,8)</f>
         <v>0x00000150</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="44"/>
-      <c r="O23" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="44"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="38"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
@@ -2396,30 +2395,30 @@
         <f t="shared" ref="B24:B31" si="1">"0x"&amp;DEC2HEX(A24,8)</f>
         <v>0x00000160</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="43"/>
-      <c r="R24" s="44"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="38"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
@@ -2429,30 +2428,30 @@
         <f t="shared" si="1"/>
         <v>0x00000170</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="L25" s="43"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="43"/>
-      <c r="R25" s="44"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="38"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
@@ -2462,30 +2461,30 @@
         <f t="shared" si="1"/>
         <v>0x00000180</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="44"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="38"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
@@ -2495,30 +2494,30 @@
         <f t="shared" si="1"/>
         <v>0x00000190</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="44"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="38"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="15">
@@ -2528,30 +2527,30 @@
         <f t="shared" si="1"/>
         <v>0x000001A0</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="L28" s="37"/>
+      <c r="M28" s="37"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="L28" s="43"/>
-      <c r="M28" s="43"/>
-      <c r="N28" s="44"/>
-      <c r="O28" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="P28" s="43"/>
-      <c r="Q28" s="43"/>
-      <c r="R28" s="44"/>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="38"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="15">
@@ -2561,30 +2560,30 @@
         <f t="shared" si="1"/>
         <v>0x000001B0</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="L29" s="37"/>
+      <c r="M29" s="37"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="P29" s="43"/>
-      <c r="Q29" s="43"/>
-      <c r="R29" s="44"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="37"/>
+      <c r="R29" s="38"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="15">
@@ -2594,30 +2593,30 @@
         <f t="shared" si="1"/>
         <v>0x000001C0</v>
       </c>
-      <c r="C30" s="42" t="s">
+      <c r="C30" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="L30" s="37"/>
+      <c r="M30" s="37"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="44"/>
-      <c r="O30" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="P30" s="43"/>
-      <c r="Q30" s="43"/>
-      <c r="R30" s="44"/>
+      <c r="P30" s="37"/>
+      <c r="Q30" s="37"/>
+      <c r="R30" s="38"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
@@ -2627,30 +2626,30 @@
         <f t="shared" si="1"/>
         <v>0x000001D0</v>
       </c>
-      <c r="C31" s="42" t="s">
+      <c r="C31" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="L31" s="37"/>
+      <c r="M31" s="37"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="43"/>
-      <c r="R31" s="44"/>
+      <c r="P31" s="37"/>
+      <c r="Q31" s="37"/>
+      <c r="R31" s="38"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
@@ -2660,30 +2659,30 @@
         <f>"0x"&amp;DEC2HEX(A32,8)</f>
         <v>0x000001E0</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="L32" s="43"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="44"/>
-      <c r="O32" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="P32" s="43"/>
-      <c r="Q32" s="43"/>
-      <c r="R32" s="44"/>
+      <c r="P32" s="37"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="38"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
@@ -2693,30 +2692,30 @@
         <f>"0x"&amp;DEC2HEX(A33,8)</f>
         <v>0x000001F0</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="44"/>
-      <c r="O33" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="P33" s="43"/>
-      <c r="Q33" s="43"/>
-      <c r="R33" s="44"/>
+      <c r="P33" s="37"/>
+      <c r="Q33" s="37"/>
+      <c r="R33" s="38"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
@@ -2726,30 +2725,30 @@
         <f t="shared" ref="B34:B43" si="2">"0x"&amp;DEC2HEX(A34,8)</f>
         <v>0x00000200</v>
       </c>
-      <c r="C34" s="42" t="s">
+      <c r="C34" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="44"/>
-      <c r="O34" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="P34" s="43"/>
-      <c r="Q34" s="43"/>
-      <c r="R34" s="44"/>
+      <c r="P34" s="37"/>
+      <c r="Q34" s="37"/>
+      <c r="R34" s="38"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="15">
@@ -2759,30 +2758,30 @@
         <f t="shared" si="2"/>
         <v>0x00000210</v>
       </c>
-      <c r="C35" s="42" t="s">
+      <c r="C35" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="44"/>
-      <c r="O35" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="P35" s="43"/>
-      <c r="Q35" s="43"/>
-      <c r="R35" s="44"/>
+      <c r="P35" s="37"/>
+      <c r="Q35" s="37"/>
+      <c r="R35" s="38"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
@@ -2792,41 +2791,41 @@
         <f t="shared" si="2"/>
         <v>0x00000220</v>
       </c>
-      <c r="C36" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="42" t="s">
+      <c r="C36" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="45" t="s">
+      <c r="L36" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="L36" s="45" t="s">
+      <c r="M36" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="M36" s="45" t="s">
+      <c r="N36" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="N36" s="45" t="s">
+      <c r="O36" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="O36" s="45" t="s">
+      <c r="P36" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="P36" s="45" t="s">
+      <c r="Q36" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="Q36" s="45" t="s">
+      <c r="R36" s="39" t="s">
         <v>89</v>
-      </c>
-      <c r="R36" s="45" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
@@ -2837,56 +2836,56 @@
         <f t="shared" si="2"/>
         <v>0x00000230</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="C37" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="45" t="s">
+      <c r="E37" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="45" t="s">
+      <c r="F37" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="F37" s="45" t="s">
+      <c r="G37" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="G37" s="45" t="s">
+      <c r="H37" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="H37" s="45" t="s">
+      <c r="I37" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="I37" s="45" t="s">
+      <c r="J37" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="J37" s="45" t="s">
+      <c r="K37" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="K37" s="45" t="s">
+      <c r="L37" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="L37" s="45" t="s">
+      <c r="M37" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="M37" s="45" t="s">
+      <c r="N37" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="N37" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="O37" s="46" t="s">
+      <c r="O37" s="40" t="s">
+        <v>211</v>
+      </c>
+      <c r="P37" s="40" t="s">
         <v>213</v>
       </c>
-      <c r="P37" s="46" t="s">
+      <c r="Q37" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="R37" s="40" t="s">
         <v>215</v>
       </c>
-      <c r="Q37" s="46" t="s">
-        <v>216</v>
-      </c>
-      <c r="R37" s="46" t="s">
-        <v>217</v>
-      </c>
       <c r="T37" s="15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
@@ -2897,34 +2896,34 @@
         <f t="shared" si="2"/>
         <v>0x00000240</v>
       </c>
-      <c r="C38" s="47" t="s">
+      <c r="C38" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="D38" s="41" t="s">
+        <v>217</v>
+      </c>
+      <c r="E38" s="41" t="s">
         <v>218</v>
       </c>
-      <c r="D38" s="47" t="s">
+      <c r="F38" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="E38" s="47" t="s">
+      <c r="G38" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="43"/>
+      <c r="M38" s="43"/>
+      <c r="N38" s="43"/>
+      <c r="O38" s="43"/>
+      <c r="P38" s="43"/>
+      <c r="Q38" s="43"/>
+      <c r="R38" s="44"/>
+      <c r="T38" s="15" t="s">
         <v>220</v>
-      </c>
-      <c r="F38" s="47" t="s">
-        <v>221</v>
-      </c>
-      <c r="G38" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="H38" s="49"/>
-      <c r="I38" s="49"/>
-      <c r="J38" s="49"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="49"/>
-      <c r="O38" s="49"/>
-      <c r="P38" s="49"/>
-      <c r="Q38" s="49"/>
-      <c r="R38" s="50"/>
-      <c r="T38" s="15" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
@@ -2935,24 +2934,24 @@
         <f t="shared" si="2"/>
         <v>0x00000250</v>
       </c>
-      <c r="C39" s="48" t="s">
-        <v>104</v>
-      </c>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="49"/>
-      <c r="O39" s="49"/>
-      <c r="P39" s="49"/>
-      <c r="Q39" s="49"/>
-      <c r="R39" s="50"/>
+      <c r="C39" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="43"/>
+      <c r="M39" s="43"/>
+      <c r="N39" s="43"/>
+      <c r="O39" s="43"/>
+      <c r="P39" s="43"/>
+      <c r="Q39" s="43"/>
+      <c r="R39" s="44"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="15">
@@ -2962,47 +2961,47 @@
         <f t="shared" si="2"/>
         <v>0x00000260</v>
       </c>
-      <c r="C40" s="48" t="s">
+      <c r="C40" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="49"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="51" t="s">
+      <c r="H40" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="H40" s="19" t="s">
+      <c r="I40" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="I40" s="19" t="s">
+      <c r="J40" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="J40" s="19" t="s">
+      <c r="K40" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="K40" s="19" t="s">
+      <c r="L40" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="L40" s="19" t="s">
+      <c r="M40" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="M40" s="19" t="s">
+      <c r="N40" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="N40" s="19" t="s">
+      <c r="O40" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="O40" s="19" t="s">
+      <c r="P40" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="P40" s="19" t="s">
+      <c r="Q40" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="Q40" s="19" t="s">
+      <c r="R40" s="49" t="s">
         <v>116</v>
-      </c>
-      <c r="R40" s="19" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
@@ -3013,53 +3012,53 @@
         <f t="shared" si="2"/>
         <v>0x00000270</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="E41" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="F41" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="F41" s="19" t="s">
+      <c r="G41" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="G41" s="19" t="s">
+      <c r="H41" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="H41" s="19" t="s">
+      <c r="I41" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="I41" s="19" t="s">
+      <c r="J41" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="J41" s="19" t="s">
+      <c r="K41" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="K41" s="19" t="s">
+      <c r="L41" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="L41" s="20" t="s">
+      <c r="M41" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="M41" s="20" t="s">
+      <c r="N41" s="50" t="s">
         <v>128</v>
       </c>
-      <c r="N41" s="20" t="s">
+      <c r="O41" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="O41" s="20" t="s">
+      <c r="P41" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="P41" s="20" t="s">
+      <c r="Q41" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="Q41" s="20" t="s">
+      <c r="R41" s="50" t="s">
         <v>132</v>
-      </c>
-      <c r="R41" s="20" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
@@ -3070,56 +3069,56 @@
         <f t="shared" si="2"/>
         <v>0x00000280</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="E42" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="E42" s="20" t="s">
+      <c r="F42" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="G42" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="G42" s="20" t="s">
+      <c r="H42" s="50" t="s">
         <v>138</v>
       </c>
-      <c r="H42" s="20" t="s">
+      <c r="I42" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="I42" s="20" t="s">
+      <c r="J42" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="J42" s="20" t="s">
+      <c r="K42" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="K42" s="20" t="s">
+      <c r="L42" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="L42" s="20" t="s">
+      <c r="M42" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="M42" s="20" t="s">
+      <c r="N42" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="N42" s="20" t="s">
+      <c r="O42" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="O42" s="20" t="s">
+      <c r="P42" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="P42" s="51" t="s">
+      <c r="Q42" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="R42" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="Q42" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="R42" s="51" t="s">
-        <v>148</v>
-      </c>
       <c r="T42" s="15" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
@@ -3130,32 +3129,32 @@
         <f t="shared" si="2"/>
         <v>0x00000290</v>
       </c>
-      <c r="C43" s="22" t="s">
+      <c r="C43" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="46" t="s">
         <v>226</v>
       </c>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="L43" s="23"/>
-      <c r="M43" s="23"/>
-      <c r="N43" s="24"/>
-      <c r="O43" s="22" t="s">
-        <v>223</v>
-      </c>
-      <c r="P43" s="23"/>
-      <c r="Q43" s="23"/>
-      <c r="R43" s="24"/>
+      <c r="L43" s="47"/>
+      <c r="M43" s="47"/>
+      <c r="N43" s="48"/>
+      <c r="O43" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="P43" s="47"/>
+      <c r="Q43" s="47"/>
+      <c r="R43" s="48"/>
       <c r="T43" s="15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
@@ -3166,30 +3165,30 @@
         <f>"0x"&amp;DEC2HEX(A44,8)</f>
         <v>0x000002A0</v>
       </c>
-      <c r="C44" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="24"/>
-      <c r="O44" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="23"/>
-      <c r="R44" s="24"/>
+      <c r="C44" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="48"/>
+      <c r="G44" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="H44" s="47"/>
+      <c r="I44" s="47"/>
+      <c r="J44" s="48"/>
+      <c r="K44" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="L44" s="47"/>
+      <c r="M44" s="47"/>
+      <c r="N44" s="48"/>
+      <c r="O44" s="46" t="s">
+        <v>228</v>
+      </c>
+      <c r="P44" s="47"/>
+      <c r="Q44" s="47"/>
+      <c r="R44" s="48"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="15">
@@ -3199,30 +3198,30 @@
         <f>"0x"&amp;DEC2HEX(A45,8)</f>
         <v>0x000002B0</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="46" t="s">
+        <v>229</v>
+      </c>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="46" t="s">
+        <v>230</v>
+      </c>
+      <c r="H45" s="47"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="46" t="s">
         <v>231</v>
       </c>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="22" t="s">
+      <c r="L45" s="47"/>
+      <c r="M45" s="47"/>
+      <c r="N45" s="48"/>
+      <c r="O45" s="46" t="s">
         <v>232</v>
       </c>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="L45" s="23"/>
-      <c r="M45" s="23"/>
-      <c r="N45" s="24"/>
-      <c r="O45" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="P45" s="23"/>
-      <c r="Q45" s="23"/>
-      <c r="R45" s="24"/>
+      <c r="P45" s="47"/>
+      <c r="Q45" s="47"/>
+      <c r="R45" s="48"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="15">
@@ -3232,30 +3231,30 @@
         <f t="shared" ref="B46" si="3">"0x"&amp;DEC2HEX(A46,8)</f>
         <v>0x000002C0</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C46" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="46" t="s">
+        <v>234</v>
+      </c>
+      <c r="H46" s="47"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="22" t="s">
+      <c r="L46" s="47"/>
+      <c r="M46" s="47"/>
+      <c r="N46" s="48"/>
+      <c r="O46" s="46" t="s">
         <v>236</v>
       </c>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="22" t="s">
-        <v>237</v>
-      </c>
-      <c r="L46" s="23"/>
-      <c r="M46" s="23"/>
-      <c r="N46" s="24"/>
-      <c r="O46" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="P46" s="23"/>
-      <c r="Q46" s="23"/>
-      <c r="R46" s="24"/>
+      <c r="P46" s="47"/>
+      <c r="Q46" s="47"/>
+      <c r="R46" s="48"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="15">
@@ -3265,30 +3264,30 @@
         <f>"0x"&amp;DEC2HEX(A47,8)</f>
         <v>0x000002D0</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="46" t="s">
+        <v>237</v>
+      </c>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="46" t="s">
+        <v>238</v>
+      </c>
+      <c r="H47" s="47"/>
+      <c r="I47" s="47"/>
+      <c r="J47" s="48"/>
+      <c r="K47" s="46" t="s">
         <v>239</v>
       </c>
-      <c r="D47" s="23"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="22" t="s">
+      <c r="L47" s="47"/>
+      <c r="M47" s="47"/>
+      <c r="N47" s="48"/>
+      <c r="O47" s="46" t="s">
         <v>240</v>
       </c>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="24"/>
-      <c r="K47" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="L47" s="23"/>
-      <c r="M47" s="23"/>
-      <c r="N47" s="24"/>
-      <c r="O47" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="P47" s="23"/>
-      <c r="Q47" s="23"/>
-      <c r="R47" s="24"/>
+      <c r="P47" s="47"/>
+      <c r="Q47" s="47"/>
+      <c r="R47" s="48"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="15">
@@ -3298,35 +3297,35 @@
         <f>"0x"&amp;DEC2HEX(A48,8)</f>
         <v>0x000002E0</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C48" s="46" t="s">
+        <v>241</v>
+      </c>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="H48" s="47"/>
+      <c r="I48" s="47"/>
+      <c r="J48" s="48"/>
+      <c r="K48" s="46" t="s">
         <v>243</v>
       </c>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="22" t="s">
+      <c r="L48" s="47"/>
+      <c r="M48" s="47"/>
+      <c r="N48" s="48"/>
+      <c r="O48" s="46" t="s">
         <v>244</v>
       </c>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="24"/>
-      <c r="K48" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="L48" s="23"/>
-      <c r="M48" s="23"/>
-      <c r="N48" s="24"/>
-      <c r="O48" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="P48" s="23"/>
-      <c r="Q48" s="23"/>
-      <c r="R48" s="24"/>
+      <c r="P48" s="47"/>
+      <c r="Q48" s="47"/>
+      <c r="R48" s="48"/>
     </row>
     <row r="51" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S51" s="18"/>
       <c r="T51" s="15" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -3515,42 +3514,42 @@
   <sheetData>
     <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="32" t="s">
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="35" t="s">
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="1">

</xml_diff>